<commit_message>
chore: contamination, delete segmented models, replace by spearman's tests => metals
</commit_message>
<xml_diff>
--- a/inst/results/data_contam/metals/general_eval_metals_µg_ww.xlsx
+++ b/inst/results/data_contam/metals/general_eval_metals_µg_ww.xlsx
@@ -383,44 +383,44 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mercure</t>
+          <t>Cadmium</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>→  →  blue</t>
+          <t>↓  →  orange</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>→  →  blue</t>
+          <t>↓  ↓  blue</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>→  →  blue</t>
+          <t>↓  →  blue</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cadmium</t>
+          <t>Mercure</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>↓  →  orange</t>
+          <t>→  →  blue</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>↓  →  blue</t>
+          <t>→  →  blue</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>↓  →  blue</t>
+          <t>→  →  blue</t>
         </is>
       </c>
     </row>
@@ -437,12 +437,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>↓  →  blue</t>
+          <t>↓  ↓  blue</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>→  ↓  blue</t>
+          <t>→  →  blue</t>
         </is>
       </c>
     </row>
@@ -453,7 +453,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -472,50 +472,45 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>break_dates</t>
+          <t>rho</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>last_p_value</t>
+          <t>p.value</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>last_slope</t>
+          <t>short_last_trend</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>short_last_trend</t>
+          <t>EC_MPC_µg_gww</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>EC_MPC_µg_gww</t>
+          <t>pvalue</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>pvalue</t>
+          <t>median_1</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>median_1</t>
+          <t>median_2</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>median_2</t>
+          <t>long_term_trend</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>long_term_trend</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
@@ -529,52 +524,49 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mercure</t>
+          <t>Cadmium</t>
         </is>
       </c>
       <c r="C2">
-        <v>2003.999522268946</v>
+        <v>-0.04642857142857142</v>
       </c>
       <c r="D2">
-        <v>0.1756492873533557</v>
-      </c>
-      <c r="E2">
-        <v>0.00023947</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G2">
-        <v>0.5</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0.206</t>
-        </is>
+        <v>0.8726807323661729</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.0019</t>
+        </is>
+      </c>
+      <c r="H2">
+        <v>772</v>
       </c>
       <c r="I2">
-        <v>3.2</v>
-      </c>
-      <c r="J2">
-        <v>3.6</v>
+        <v>240.7</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>blue</t>
+          <t>orange</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Loire</t>
+          <t>Gironde</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -583,39 +575,36 @@
         </is>
       </c>
       <c r="C3">
-        <v>2012.0001</v>
+        <v>-0.1982062417930229</v>
       </c>
       <c r="D3">
-        <v>0.5535354163385215</v>
-      </c>
-      <c r="E3">
-        <v>0.00024521</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G3">
+        <v>0.4788663786637513</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="F3">
         <v>0.5</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0.187</t>
-        </is>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.206</t>
+        </is>
+      </c>
+      <c r="H3">
+        <v>3.2</v>
       </c>
       <c r="I3">
-        <v>3.8</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
+        <v>3.6</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
       </c>
       <c r="K3" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
         <is>
           <t>blue</t>
         </is>
@@ -624,48 +613,45 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Seine</t>
+          <t>Gironde</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mercure</t>
+          <t>Plomb</t>
         </is>
       </c>
       <c r="C4">
-        <v>2019.999951308937</v>
+        <v>0.3821428571428571</v>
       </c>
       <c r="D4">
-        <v>0.2134755381806601</v>
-      </c>
-      <c r="E4">
-        <v>0.0045443</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G4">
-        <v>0.5</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
+        <v>0.1606519299640411</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="F4">
+        <v>1.5</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.0523</t>
+        </is>
+      </c>
+      <c r="H4">
+        <v>21.53</v>
       </c>
       <c r="I4">
-        <v>9.9</v>
-      </c>
-      <c r="J4">
-        <v>7.6</v>
+        <v>25.6</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
       </c>
       <c r="K4" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
         <is>
           <t>blue</t>
         </is>
@@ -674,7 +660,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Gironde</t>
+          <t>Loire</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -683,41 +669,38 @@
         </is>
       </c>
       <c r="C5">
-        <v>2007.646046953573</v>
+        <v>-0.5438770451165098</v>
       </c>
       <c r="D5">
-        <v>0.7660697079983512</v>
-      </c>
-      <c r="E5">
-        <v>-0.013046</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G5">
+        <v>0.00730453556966146</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>0.0019</t>
-        </is>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.00876</t>
+        </is>
+      </c>
+      <c r="H5">
+        <v>27.85</v>
       </c>
       <c r="I5">
-        <v>772</v>
-      </c>
-      <c r="J5">
-        <v>240.7</v>
+        <v>18.3</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>orange</t>
+          <t>blue</t>
         </is>
       </c>
     </row>
@@ -729,43 +712,40 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cadmium</t>
+          <t>Mercure</t>
         </is>
       </c>
       <c r="C6">
-        <v>1988.000008571352</v>
+        <v>0.01577256784261706</v>
       </c>
       <c r="D6">
-        <v>0.3073246210577655</v>
-      </c>
-      <c r="E6">
-        <v>-0.00075324</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>0.00876</t>
-        </is>
+        <v>0.9340709733948784</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="F6">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0.187</t>
+        </is>
+      </c>
+      <c r="H6">
+        <v>3.8</v>
       </c>
       <c r="I6">
-        <v>27.85</v>
-      </c>
-      <c r="J6">
-        <v>18.3</v>
+        <v>5</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
       </c>
       <c r="K6" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
         <is>
           <t>blue</t>
         </is>
@@ -774,48 +754,45 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Seine</t>
+          <t>Loire</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cadmium</t>
+          <t>Plomb</t>
         </is>
       </c>
       <c r="C7">
-        <v>1997.340317676886</v>
+        <v>-0.6321269211700545</v>
       </c>
       <c r="D7">
-        <v>0.9446611629794449</v>
-      </c>
-      <c r="E7">
-        <v>-0.00029384</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>0.0105</t>
-        </is>
+        <v>0.001212216103966395</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="F7">
+        <v>1.5</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.000878</t>
+        </is>
+      </c>
+      <c r="H7">
+        <v>57.73</v>
       </c>
       <c r="I7">
-        <v>67.84999999999999</v>
-      </c>
-      <c r="J7">
-        <v>25.95</v>
+        <v>13.67</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
       </c>
       <c r="K7" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
         <is>
           <t>blue</t>
         </is>
@@ -824,48 +801,45 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Gironde</t>
+          <t>Seine</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Plomb</t>
+          <t>Cadmium</t>
         </is>
       </c>
       <c r="C8">
-        <v>2008.000018099827</v>
+        <v>-0.3538461538461539</v>
       </c>
       <c r="D8">
-        <v>0.09667735816216919</v>
-      </c>
-      <c r="E8">
-        <v>0.0061026</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G8">
-        <v>1.5</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>0.0523</t>
-        </is>
+        <v>0.214890520556095</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.0105</t>
+        </is>
+      </c>
+      <c r="H8">
+        <v>67.84999999999999</v>
       </c>
       <c r="I8">
-        <v>21.53</v>
-      </c>
-      <c r="J8">
-        <v>25.6</v>
+        <v>25.95</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
       </c>
       <c r="K8" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
         <is>
           <t>blue</t>
         </is>
@@ -874,48 +848,45 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Loire</t>
+          <t>Seine</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Plomb</t>
+          <t>Mercure</t>
         </is>
       </c>
       <c r="C9">
-        <v>2003.496772800662</v>
+        <v>-0.1097966354784204</v>
       </c>
       <c r="D9">
-        <v>0.1558042743392387</v>
-      </c>
-      <c r="E9">
-        <v>-0.0036628</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G9">
-        <v>1.5</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>0.000878</t>
-        </is>
+        <v>0.6856331238400547</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="F9">
+        <v>0.5</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="H9">
+        <v>9.9</v>
       </c>
       <c r="I9">
-        <v>57.73</v>
-      </c>
-      <c r="J9">
-        <v>13.67</v>
+        <v>7.6</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
       </c>
       <c r="K9" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
         <is>
           <t>blue</t>
         </is>
@@ -933,39 +904,36 @@
         </is>
       </c>
       <c r="C10">
-        <v>1996.461899140737</v>
+        <v>-0.4796482550418079</v>
       </c>
       <c r="D10">
-        <v>8.616131854373594E-07</v>
-      </c>
-      <c r="E10">
-        <v>-0.018297</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="G10">
+        <v>0.08263542281872624</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="F10">
         <v>1.5</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>0.0881</t>
         </is>
       </c>
+      <c r="H10">
+        <v>42.23</v>
+      </c>
       <c r="I10">
-        <v>42.23</v>
-      </c>
-      <c r="J10">
         <v>31.5</v>
       </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
         <is>
           <t>blue</t>
         </is>

</xml_diff>